<commit_message>
Updated OLR wrangling, ready for test ingest
</commit_message>
<xml_diff>
--- a/mss0080/OLR/xls_standard_input_template_MSS0080.xlsx
+++ b/mss0080/OLR/xls_standard_input_template_MSS0080.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\small_manuscript_collections\mss0080\Working_metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\domm-metadata\mss0080\OLR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26040" windowHeight="9210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26040" windowHeight="9210" tabRatio="381"/>
   </bookViews>
   <sheets>
     <sheet name="Item description" sheetId="9" r:id="rId1"/>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="968">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="968">
   <si>
     <t>text</t>
   </si>
@@ -4114,12 +4114,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X44"/>
+  <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="M3" sqref="M1:M1048576"/>
+      <selection pane="bottomLeft" activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4144,10 +4144,9 @@
     <col min="19" max="19" width="16" style="3" customWidth="1"/>
     <col min="20" max="20" width="22.42578125" style="3" customWidth="1"/>
     <col min="21" max="21" width="42.85546875" style="3" customWidth="1"/>
-    <col min="22" max="22" width="84.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>338</v>
       </c>
@@ -4211,11 +4210,8 @@
       <c r="U1" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="V1" s="16" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>842</v>
       </c>
@@ -4271,9 +4267,8 @@
         <v>888</v>
       </c>
       <c r="U2" s="23"/>
-      <c r="V2" s="25"/>
-    </row>
-    <row r="3" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>843</v>
       </c>
@@ -4327,9 +4322,8 @@
       </c>
       <c r="T3" s="23"/>
       <c r="U3" s="23"/>
-      <c r="V3" s="25"/>
-    </row>
-    <row r="4" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>844</v>
       </c>
@@ -4383,9 +4377,8 @@
       <c r="U4" s="23" t="s">
         <v>959</v>
       </c>
-      <c r="V4" s="25"/>
-    </row>
-    <row r="5" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>845</v>
       </c>
@@ -4443,9 +4436,8 @@
       <c r="U5" s="23" t="s">
         <v>962</v>
       </c>
-      <c r="V5" s="25"/>
-    </row>
-    <row r="6" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>846</v>
       </c>
@@ -4503,9 +4495,8 @@
       <c r="U6" s="23" t="s">
         <v>959</v>
       </c>
-      <c r="V6" s="25"/>
-    </row>
-    <row r="7" spans="1:22" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:21" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>847</v>
       </c>
@@ -4565,9 +4556,8 @@
       <c r="U7" s="23" t="s">
         <v>965</v>
       </c>
-      <c r="V7" s="25"/>
-    </row>
-    <row r="8" spans="1:22" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:21" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>848</v>
       </c>
@@ -4625,9 +4615,8 @@
       <c r="U8" s="23" t="s">
         <v>957</v>
       </c>
-      <c r="V8" s="25"/>
-    </row>
-    <row r="9" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>849</v>
       </c>
@@ -4685,9 +4674,8 @@
       <c r="U9" s="23" t="s">
         <v>963</v>
       </c>
-      <c r="V9" s="25"/>
-    </row>
-    <row r="10" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>850</v>
       </c>
@@ -4745,9 +4733,8 @@
       <c r="U10" s="23" t="s">
         <v>963</v>
       </c>
-      <c r="V10" s="25"/>
-    </row>
-    <row r="11" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>851</v>
       </c>
@@ -4804,9 +4791,8 @@
       <c r="U11" s="23" t="s">
         <v>964</v>
       </c>
-      <c r="V11" s="25"/>
-    </row>
-    <row r="12" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>852</v>
       </c>
@@ -4862,9 +4848,8 @@
       <c r="U12" s="23" t="s">
         <v>964</v>
       </c>
-      <c r="V12" s="25"/>
-    </row>
-    <row r="13" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>853</v>
       </c>
@@ -4920,9 +4905,8 @@
       <c r="U13" s="23" t="s">
         <v>959</v>
       </c>
-      <c r="V13" s="25"/>
-    </row>
-    <row r="14" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>854</v>
       </c>
@@ -4976,9 +4960,8 @@
       <c r="U14" s="23" t="s">
         <v>964</v>
       </c>
-      <c r="V14" s="25"/>
-    </row>
-    <row r="15" spans="1:22" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:21" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>855</v>
       </c>
@@ -5032,9 +5015,8 @@
       <c r="U15" s="23" t="s">
         <v>957</v>
       </c>
-      <c r="V15" s="25"/>
-    </row>
-    <row r="16" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>856</v>
       </c>
@@ -5090,9 +5072,8 @@
       <c r="U16" s="23" t="s">
         <v>964</v>
       </c>
-      <c r="V16" s="25"/>
-    </row>
-    <row r="17" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>857</v>
       </c>
@@ -5150,9 +5131,8 @@
       <c r="U17" s="23" t="s">
         <v>964</v>
       </c>
-      <c r="V17" s="25"/>
-    </row>
-    <row r="18" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>858</v>
       </c>
@@ -5208,9 +5188,8 @@
       <c r="U18" s="23" t="s">
         <v>964</v>
       </c>
-      <c r="V18" s="25"/>
-    </row>
-    <row r="19" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>859</v>
       </c>
@@ -5266,9 +5245,8 @@
       <c r="U19" s="23" t="s">
         <v>964</v>
       </c>
-      <c r="V19" s="25"/>
-    </row>
-    <row r="20" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>860</v>
       </c>
@@ -5324,9 +5302,8 @@
       <c r="U20" s="23" t="s">
         <v>964</v>
       </c>
-      <c r="V20" s="25"/>
-    </row>
-    <row r="21" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>861</v>
       </c>
@@ -5382,9 +5359,8 @@
       <c r="U21" s="23" t="s">
         <v>964</v>
       </c>
-      <c r="V21" s="25"/>
-    </row>
-    <row r="22" spans="1:22" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:21" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>862</v>
       </c>
@@ -5440,9 +5416,8 @@
       <c r="U22" s="23" t="s">
         <v>957</v>
       </c>
-      <c r="V22" s="25"/>
-    </row>
-    <row r="23" spans="1:22" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:21" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>863</v>
       </c>
@@ -5498,9 +5473,8 @@
       <c r="U23" s="23" t="s">
         <v>957</v>
       </c>
-      <c r="V23" s="25"/>
-    </row>
-    <row r="24" spans="1:22" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:21" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>864</v>
       </c>
@@ -5558,9 +5532,8 @@
       <c r="U24" s="23" t="s">
         <v>957</v>
       </c>
-      <c r="V24" s="25"/>
-    </row>
-    <row r="25" spans="1:22" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:21" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>865</v>
       </c>
@@ -5614,9 +5587,8 @@
       <c r="U25" s="23" t="s">
         <v>960</v>
       </c>
-      <c r="V25" s="25"/>
-    </row>
-    <row r="26" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>866</v>
       </c>
@@ -5676,9 +5648,8 @@
       <c r="U26" s="23" t="s">
         <v>961</v>
       </c>
-      <c r="V26" s="25"/>
-    </row>
-    <row r="27" spans="1:22" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:21" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
         <v>867</v>
       </c>
@@ -5736,9 +5707,8 @@
       <c r="U27" s="23" t="s">
         <v>960</v>
       </c>
-      <c r="V27" s="25"/>
-    </row>
-    <row r="28" spans="1:22" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:21" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
         <v>868</v>
       </c>
@@ -5798,9 +5768,8 @@
       <c r="U28" s="23" t="s">
         <v>957</v>
       </c>
-      <c r="V28" s="25"/>
-    </row>
-    <row r="29" spans="1:22" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:21" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>869</v>
       </c>
@@ -5856,9 +5825,8 @@
       <c r="U29" s="23" t="s">
         <v>960</v>
       </c>
-      <c r="V29" s="25"/>
-    </row>
-    <row r="30" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
         <v>870</v>
       </c>
@@ -5918,9 +5886,8 @@
       <c r="U30" s="23" t="s">
         <v>961</v>
       </c>
-      <c r="V30" s="25"/>
-    </row>
-    <row r="31" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
         <v>871</v>
       </c>
@@ -5978,9 +5945,8 @@
       <c r="U31" s="23" t="s">
         <v>959</v>
       </c>
-      <c r="V31" s="25"/>
-    </row>
-    <row r="32" spans="1:22" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:21" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
         <v>872</v>
       </c>
@@ -6040,9 +6006,8 @@
       <c r="U32" s="23" t="s">
         <v>957</v>
       </c>
-      <c r="V32" s="25"/>
-    </row>
-    <row r="33" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
         <v>873</v>
       </c>
@@ -6102,9 +6067,8 @@
       <c r="U33" s="23" t="s">
         <v>961</v>
       </c>
-      <c r="V33" s="25"/>
-    </row>
-    <row r="34" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
         <v>874</v>
       </c>
@@ -6162,9 +6126,8 @@
       <c r="U34" s="23" t="s">
         <v>961</v>
       </c>
-      <c r="V34" s="25"/>
-    </row>
-    <row r="35" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
         <v>875</v>
       </c>
@@ -6224,9 +6187,8 @@
       <c r="U35" s="23" t="s">
         <v>961</v>
       </c>
-      <c r="V35" s="25"/>
-    </row>
-    <row r="36" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
         <v>876</v>
       </c>
@@ -6282,9 +6244,8 @@
       <c r="U36" s="23" t="s">
         <v>961</v>
       </c>
-      <c r="V36" s="25"/>
-    </row>
-    <row r="37" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>877</v>
       </c>
@@ -6340,9 +6301,8 @@
       <c r="U37" s="23" t="s">
         <v>961</v>
       </c>
-      <c r="V37" s="25"/>
-    </row>
-    <row r="38" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
         <v>878</v>
       </c>
@@ -6398,9 +6358,8 @@
       <c r="U38" s="23" t="s">
         <v>961</v>
       </c>
-      <c r="V38" s="25"/>
-    </row>
-    <row r="39" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
         <v>879</v>
       </c>
@@ -6456,9 +6415,8 @@
       <c r="U39" s="23" t="s">
         <v>961</v>
       </c>
-      <c r="V39" s="25"/>
-    </row>
-    <row r="40" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
         <v>880</v>
       </c>
@@ -6516,9 +6474,8 @@
       <c r="U40" s="23" t="s">
         <v>961</v>
       </c>
-      <c r="V40" s="25"/>
-    </row>
-    <row r="41" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
         <v>881</v>
       </c>
@@ -6576,9 +6533,8 @@
       <c r="U41" s="23" t="s">
         <v>961</v>
       </c>
-      <c r="V41" s="25"/>
-    </row>
-    <row r="42" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
         <v>882</v>
       </c>
@@ -6636,9 +6592,8 @@
       <c r="U42" s="23" t="s">
         <v>961</v>
       </c>
-      <c r="V42" s="25"/>
-    </row>
-    <row r="43" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
         <v>883</v>
       </c>
@@ -6696,9 +6651,8 @@
       <c r="U43" s="23" t="s">
         <v>961</v>
       </c>
-      <c r="V43" s="25"/>
-    </row>
-    <row r="44" spans="1:22" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:21" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
         <v>884</v>
       </c>
@@ -6754,7 +6708,6 @@
       <c r="U44" s="23" t="s">
         <v>961</v>
       </c>
-      <c r="V44" s="25"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
@@ -6783,7 +6736,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="12">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$A$1:$A$7</xm:f>
@@ -6801,12 +6754,6 @@
             <xm:f>'Select-a-header values'!$D$1:$D$6</xm:f>
           </x14:formula1>
           <xm:sqref>M1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
-            <xm:f>'Select-a-header values'!$I$1:$I$12</xm:f>
-          </x14:formula1>
-          <xm:sqref>V1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>

</xml_diff>